<commit_message>
still no properly working filter...
</commit_message>
<xml_diff>
--- a/data/HSK_vocabulary.xlsx
+++ b/data/HSK_vocabulary.xlsx
@@ -12,6 +12,7 @@
     <sheet name="HSK_2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="HSK_3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="TEST" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="TEST_2" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="1781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1791">
   <si>
     <t xml:space="preserve">char</t>
   </si>
@@ -181,6 +182,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">这</t>
     </r>
@@ -200,6 +202,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">这儿</t>
     </r>
@@ -217,6 +220,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">那</t>
     </r>
@@ -236,6 +240,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">那儿</t>
     </r>
@@ -253,6 +258,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">哪</t>
     </r>
@@ -272,6 +278,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">哪儿</t>
     </r>
@@ -1513,6 +1520,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">这</t>
     </r>
@@ -1532,6 +1540,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">这儿</t>
     </r>
@@ -1543,6 +1552,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">那</t>
     </r>
@@ -1562,6 +1572,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">那儿</t>
     </r>
@@ -1573,6 +1584,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">哪</t>
     </r>
@@ -1592,6 +1604,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">哪儿</t>
     </r>
@@ -1612,6 +1625,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">现在</t>
     </r>
@@ -1621,6 +1635,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -1809,6 +1824,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">茶 </t>
     </r>
@@ -1818,6 +1834,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2507,6 +2524,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">准备</t>
     </r>
@@ -4611,6 +4629,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">准备</t>
     </r>
@@ -5379,6 +5398,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">再 </t>
     </r>
@@ -5388,6 +5408,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -5468,6 +5489,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一起</t>
     </r>
@@ -5477,6 +5499,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -5569,6 +5592,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">向</t>
     </r>
@@ -5578,6 +5602,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -5589,6 +5614,7 @@
         <color rgb="FFFF6900"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">离</t>
     </r>
@@ -5598,6 +5624,7 @@
         <color rgb="FF3A3A3A"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -5761,6 +5788,36 @@
   </si>
   <si>
     <t xml:space="preserve">of course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baba is…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potato means…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a is just a letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f is also just a letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">酋批</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nowei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no way</t>
   </si>
 </sst>
 </file>
@@ -5806,6 +5863,7 @@
       <color rgb="FF3A3A3A"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="17"/>
@@ -5819,6 +5877,7 @@
       <color rgb="FFFF6900"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="17"/>
@@ -5832,6 +5891,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="17"/>
@@ -17666,16 +17726,95 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.36"/>
   </cols>
@@ -17768,8 +17907,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
main logic now finished, filtering works properly!
</commit_message>
<xml_diff>
--- a/data/HSK_vocabulary.xlsx
+++ b/data/HSK_vocabulary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HSK_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1803">
   <si>
     <t xml:space="preserve">char</t>
   </si>
@@ -2960,6 +2960,9 @@
     <t xml:space="preserve">half</t>
   </si>
   <si>
+    <t xml:space="preserve">它</t>
+  </si>
+  <si>
     <t xml:space="preserve">自己</t>
   </si>
   <si>
@@ -2987,7 +2990,7 @@
     <t xml:space="preserve">other people</t>
   </si>
   <si>
-    <t xml:space="preserve">现在  </t>
+    <t xml:space="preserve">现在</t>
   </si>
   <si>
     <t xml:space="preserve">刚才</t>
@@ -2999,6 +3002,12 @@
     <t xml:space="preserve">just now</t>
   </si>
   <si>
+    <t xml:space="preserve">小时</t>
+  </si>
+  <si>
+    <t xml:space="preserve">星期</t>
+  </si>
+  <si>
     <t xml:space="preserve">周末</t>
   </si>
   <si>
@@ -3266,7 +3275,10 @@
     <t xml:space="preserve">sound or voice</t>
   </si>
   <si>
-    <t xml:space="preserve">茶  </t>
+    <t xml:space="preserve">东西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶</t>
   </si>
   <si>
     <t xml:space="preserve">面包</t>
@@ -3821,6 +3833,9 @@
     <t xml:space="preserve">level or standard</t>
   </si>
   <si>
+    <t xml:space="preserve">事情</t>
+  </si>
+  <si>
     <t xml:space="preserve">兴趣</t>
   </si>
   <si>
@@ -4455,6 +4470,9 @@
     <t xml:space="preserve">to forget</t>
   </si>
   <si>
+    <t xml:space="preserve">让</t>
+  </si>
+  <si>
     <t xml:space="preserve">使</t>
   </si>
   <si>
@@ -4471,6 +4489,9 @@
   </si>
   <si>
     <t xml:space="preserve">to use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">希望</t>
   </si>
   <si>
     <t xml:space="preserve">帮忙</t>
@@ -5008,6 +5029,9 @@
     <t xml:space="preserve">to blow (wind)</t>
   </si>
   <si>
+    <t xml:space="preserve">好</t>
+  </si>
+  <si>
     <t xml:space="preserve">坏</t>
   </si>
   <si>
@@ -5392,26 +5416,10 @@
     <t xml:space="preserve">how…</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FFFF6900"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">再 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FF3A3A3A"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">每</t>
+  </si>
+  <si>
+    <t xml:space="preserve">再</t>
   </si>
   <si>
     <t xml:space="preserve">又</t>
@@ -5465,6 +5473,9 @@
     <t xml:space="preserve">xiān</t>
   </si>
   <si>
+    <t xml:space="preserve">已经</t>
+  </si>
+  <si>
     <t xml:space="preserve">几乎</t>
   </si>
   <si>
@@ -5483,26 +5494,7 @@
     <t xml:space="preserve">definitely</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FFFF6900"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">一起</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FF3A3A3A"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
+    <t xml:space="preserve">一起</t>
   </si>
   <si>
     <t xml:space="preserve">一共</t>
@@ -5514,6 +5506,9 @@
     <t xml:space="preserve">altogether</t>
   </si>
   <si>
+    <t xml:space="preserve">可能</t>
+  </si>
+  <si>
     <t xml:space="preserve">其实</t>
   </si>
   <si>
@@ -5586,48 +5581,13 @@
     <t xml:space="preserve">constantly</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FFFF6900"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">向</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FF3A3A3A"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FFFF6900"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">离</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color rgb="FF3A3A3A"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">从</t>
+  </si>
+  <si>
+    <t xml:space="preserve">向</t>
+  </si>
+  <si>
+    <t xml:space="preserve">离</t>
   </si>
   <si>
     <t xml:space="preserve">跟</t>
@@ -11087,8 +11047,8 @@
   </sheetPr>
   <dimension ref="A1:C601"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11354,7 +11314,7 @@
     </row>
     <row r="24" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>462</v>
+        <v>901</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>43</v>
@@ -11376,13 +11336,13 @@
     </row>
     <row r="26" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11398,24 +11358,24 @@
     </row>
     <row r="28" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11530,7 +11490,7 @@
     </row>
     <row r="40" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>77</v>
@@ -11541,13 +11501,13 @@
     </row>
     <row r="41" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11651,7 +11611,7 @@
     </row>
     <row r="51" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>480</v>
+        <v>915</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>481</v>
@@ -11717,7 +11677,7 @@
     </row>
     <row r="57" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>486</v>
+        <v>916</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>113</v>
@@ -11728,13 +11688,13 @@
     </row>
     <row r="58" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11761,57 +11721,57 @@
     </row>
     <row r="61" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11827,68 +11787,68 @@
     </row>
     <row r="67" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>938</v>
+        <v>941</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>254</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12069,46 +12029,46 @@
     </row>
     <row r="89" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>955</v>
+        <v>958</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12124,24 +12084,24 @@
     </row>
     <row r="94" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12201,24 +12161,24 @@
     </row>
     <row r="101" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>967</v>
+        <v>970</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12234,13 +12194,13 @@
     </row>
     <row r="104" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>973</v>
+        <v>976</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>974</v>
+        <v>977</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>975</v>
+        <v>978</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12256,13 +12216,13 @@
     </row>
     <row r="106" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>978</v>
+        <v>981</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12278,13 +12238,13 @@
     </row>
     <row r="108" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12300,84 +12260,84 @@
     </row>
     <row r="110" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>984</v>
+        <v>987</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>985</v>
+        <v>988</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>987</v>
+        <v>990</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>988</v>
+        <v>991</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>989</v>
+        <v>992</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4" t="s">
-        <v>532</v>
+        <v>1006</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>158</v>
@@ -12410,7 +12370,7 @@
     </row>
     <row r="120" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>167</v>
@@ -12443,35 +12403,35 @@
     </row>
     <row r="123" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12498,13 +12458,13 @@
     </row>
     <row r="128" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>1015</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12542,13 +12502,13 @@
     </row>
     <row r="132" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12564,101 +12524,101 @@
     </row>
     <row r="134" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>1021</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>1024</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>1033</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>1036</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>1042</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>1043</v>
+        <v>1047</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>1044</v>
+        <v>1048</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>1045</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12685,24 +12645,24 @@
     </row>
     <row r="145" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>1046</v>
+        <v>1050</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>1047</v>
+        <v>1051</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>1048</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>1049</v>
+        <v>1053</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1050</v>
+        <v>1054</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>1051</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12718,46 +12678,46 @@
     </row>
     <row r="148" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>1052</v>
+        <v>1056</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1053</v>
+        <v>1057</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>1054</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>1055</v>
+        <v>1059</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
-        <v>1058</v>
+        <v>1062</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1059</v>
+        <v>1063</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>1060</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>1061</v>
+        <v>1065</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1062</v>
+        <v>1066</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>1063</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12765,7 +12725,7 @@
         <v>181</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>1064</v>
+        <v>1068</v>
       </c>
       <c r="C152" s="5" t="s">
         <v>183</v>
@@ -12784,24 +12744,24 @@
     </row>
     <row r="154" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
-        <v>1065</v>
+        <v>1069</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
-        <v>1068</v>
+        <v>1072</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1069</v>
+        <v>1073</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>1070</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12828,13 +12788,13 @@
     </row>
     <row r="158" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>1071</v>
+        <v>1075</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1072</v>
+        <v>1076</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>1073</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12850,46 +12810,46 @@
     </row>
     <row r="160" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>1074</v>
+        <v>1078</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1075</v>
+        <v>1079</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>1076</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>1077</v>
+        <v>1081</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1078</v>
+        <v>1082</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>1079</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>1080</v>
+        <v>1084</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1081</v>
+        <v>1085</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>1083</v>
+        <v>1087</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1084</v>
+        <v>1088</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>1085</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12916,35 +12876,35 @@
     </row>
     <row r="166" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>1086</v>
+        <v>1090</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1087</v>
+        <v>1091</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>1088</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>1089</v>
+        <v>1093</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1090</v>
+        <v>1094</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>1091</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>1092</v>
+        <v>1096</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>1094</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12993,46 +12953,46 @@
     </row>
     <row r="173" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>1095</v>
+        <v>1099</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>1097</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>1098</v>
+        <v>1102</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1099</v>
+        <v>1103</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>1100</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>1101</v>
+        <v>1105</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1102</v>
+        <v>1106</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>1103</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13040,7 +13000,7 @@
         <v>202</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
       <c r="C177" s="5" t="s">
         <v>204</v>
@@ -13048,13 +13008,13 @@
     </row>
     <row r="178" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>1110</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13062,7 +13022,7 @@
         <v>205</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>1111</v>
+        <v>1115</v>
       </c>
       <c r="C179" s="5" t="s">
         <v>207</v>
@@ -13092,13 +13052,13 @@
     </row>
     <row r="182" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>1114</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13136,13 +13096,13 @@
     </row>
     <row r="186" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>1115</v>
+        <v>1119</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13158,13 +13118,13 @@
     </row>
     <row r="188" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>1118</v>
+        <v>1122</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1119</v>
+        <v>1123</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>1120</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13191,46 +13151,46 @@
     </row>
     <row r="191" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>1121</v>
+        <v>1125</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1122</v>
+        <v>1126</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>1123</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>1124</v>
+        <v>1128</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1125</v>
+        <v>1129</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>1126</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>1127</v>
+        <v>1131</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1128</v>
+        <v>1132</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>1129</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>1130</v>
+        <v>1134</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1131</v>
+        <v>1135</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>1132</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13246,35 +13206,35 @@
     </row>
     <row r="196" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>1133</v>
+        <v>1137</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1134</v>
+        <v>1138</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>1135</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>1136</v>
+        <v>1140</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1137</v>
+        <v>1141</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>1138</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>1139</v>
+        <v>1143</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1140</v>
+        <v>1144</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>1141</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13301,24 +13261,24 @@
     </row>
     <row r="201" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>1142</v>
+        <v>1146</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1143</v>
+        <v>1147</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>1144</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>1145</v>
+        <v>1149</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1146</v>
+        <v>1150</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>1147</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13334,24 +13294,24 @@
     </row>
     <row r="204" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
-        <v>1148</v>
+        <v>1152</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>1149</v>
+        <v>1153</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>1150</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>1153</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13367,35 +13327,35 @@
     </row>
     <row r="207" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="2" t="s">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1155</v>
+        <v>1159</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>1156</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
-        <v>1157</v>
+        <v>1161</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1158</v>
+        <v>1162</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>1159</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="2" t="s">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>1161</v>
+        <v>1165</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>1162</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13411,24 +13371,24 @@
     </row>
     <row r="211" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="2" t="s">
-        <v>1163</v>
+        <v>1167</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>1164</v>
+        <v>1168</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>1165</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="2" t="s">
-        <v>1166</v>
+        <v>1170</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>1167</v>
+        <v>1171</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>1168</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13466,7 +13426,7 @@
     </row>
     <row r="216" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="4" t="s">
-        <v>601</v>
+        <v>1173</v>
       </c>
       <c r="B216" s="5" t="s">
         <v>602</v>
@@ -13477,211 +13437,211 @@
     </row>
     <row r="217" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="2" t="s">
-        <v>1169</v>
+        <v>1174</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1170</v>
+        <v>1175</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>1171</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="s">
-        <v>1172</v>
+        <v>1177</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>1173</v>
+        <v>1178</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>1174</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="s">
-        <v>1175</v>
+        <v>1180</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>1176</v>
+        <v>1181</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>1177</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="s">
-        <v>1178</v>
+        <v>1183</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>1179</v>
+        <v>1184</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>1180</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
-        <v>1181</v>
+        <v>1186</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>1182</v>
+        <v>1187</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>1183</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="s">
-        <v>1184</v>
+        <v>1189</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>1185</v>
+        <v>1190</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>1186</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
-        <v>1187</v>
+        <v>1192</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>1188</v>
+        <v>1193</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>1189</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
-        <v>1190</v>
+        <v>1195</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>1191</v>
+        <v>1196</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>1192</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
-        <v>1193</v>
+        <v>1198</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1194</v>
+        <v>1199</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>1195</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
-        <v>1196</v>
+        <v>1201</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>1197</v>
+        <v>1202</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>1198</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
-        <v>1199</v>
+        <v>1204</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>1200</v>
+        <v>1205</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>1201</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
-        <v>1202</v>
+        <v>1207</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1203</v>
+        <v>1208</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>1204</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="s">
-        <v>1205</v>
+        <v>1210</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>1206</v>
+        <v>1211</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>1207</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
-        <v>1208</v>
+        <v>1213</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>1209</v>
+        <v>1214</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>1210</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="s">
-        <v>1211</v>
+        <v>1216</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>1212</v>
+        <v>1217</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>1213</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="s">
-        <v>1214</v>
+        <v>1219</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>1215</v>
+        <v>1220</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>1216</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
-        <v>1217</v>
+        <v>1222</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>1218</v>
+        <v>1223</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>1219</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="s">
-        <v>1220</v>
+        <v>1225</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>1221</v>
+        <v>1226</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>1222</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
-        <v>1223</v>
+        <v>1228</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1224</v>
+        <v>1229</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>1225</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13708,35 +13668,35 @@
     </row>
     <row r="238" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>1226</v>
+        <v>1231</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>1227</v>
+        <v>1232</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>1228</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>1229</v>
+        <v>1234</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>1230</v>
+        <v>1235</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>1231</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>1232</v>
+        <v>1237</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>1233</v>
+        <v>1238</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>1234</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13752,13 +13712,13 @@
     </row>
     <row r="242" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>1235</v>
+        <v>1240</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1236</v>
+        <v>1241</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>1237</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13774,24 +13734,24 @@
     </row>
     <row r="244" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>1238</v>
+        <v>1243</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>1239</v>
+        <v>1244</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>1240</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>1241</v>
+        <v>1246</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>1242</v>
+        <v>1247</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>1243</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13818,13 +13778,13 @@
     </row>
     <row r="248" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>1244</v>
+        <v>1249</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>1245</v>
+        <v>1250</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>1246</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13840,13 +13800,13 @@
     </row>
     <row r="250" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>1247</v>
+        <v>1252</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>1248</v>
+        <v>1253</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>1249</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13862,13 +13822,13 @@
     </row>
     <row r="252" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>1250</v>
+        <v>1255</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>1251</v>
+        <v>1256</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>1252</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13884,46 +13844,46 @@
     </row>
     <row r="254" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>1253</v>
+        <v>1258</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>1254</v>
+        <v>1259</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>1255</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>1256</v>
+        <v>1261</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>1257</v>
+        <v>1262</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>1258</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>1259</v>
+        <v>1264</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1260</v>
+        <v>1265</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>1261</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>1262</v>
+        <v>1267</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1263</v>
+        <v>1268</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>1264</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13972,24 +13932,24 @@
     </row>
     <row r="262" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>1265</v>
+        <v>1270</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1266</v>
+        <v>1271</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>1267</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>1268</v>
+        <v>1273</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>425</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>1269</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14038,13 +13998,13 @@
     </row>
     <row r="268" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>1270</v>
+        <v>1275</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1271</v>
+        <v>1276</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>1272</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14060,13 +14020,13 @@
     </row>
     <row r="270" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>1273</v>
+        <v>1278</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>1274</v>
+        <v>1279</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>1275</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14115,46 +14075,46 @@
     </row>
     <row r="275" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>1276</v>
+        <v>1281</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>1277</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>1278</v>
+        <v>1283</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>1279</v>
+        <v>1284</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>1280</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>1281</v>
+        <v>1286</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>1282</v>
+        <v>1287</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>1283</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>1284</v>
+        <v>1289</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>1285</v>
+        <v>1290</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>1286</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14192,24 +14152,24 @@
     </row>
     <row r="282" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>1287</v>
+        <v>1292</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>1288</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>1289</v>
+        <v>1294</v>
       </c>
       <c r="B283" s="3" t="s">
         <v>428</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>1290</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14228,7 +14188,7 @@
         <v>274</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>1291</v>
+        <v>1296</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>276</v>
@@ -14269,13 +14229,13 @@
     </row>
     <row r="289" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>1292</v>
+        <v>1297</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>1293</v>
+        <v>1298</v>
       </c>
       <c r="C289" s="3" t="s">
-        <v>1294</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14302,90 +14262,90 @@
     </row>
     <row r="292" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>1295</v>
+        <v>1300</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>1296</v>
+        <v>1301</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>1297</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>1298</v>
+        <v>1303</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>1299</v>
+        <v>1304</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>1300</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>1301</v>
+        <v>1306</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>1302</v>
+        <v>1307</v>
       </c>
       <c r="C294" s="3" t="s">
-        <v>1303</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>1304</v>
+        <v>1309</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>1305</v>
+        <v>1310</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>1306</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>1307</v>
+        <v>1312</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>1308</v>
+        <v>1313</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>1309</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>1310</v>
+        <v>1315</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>1311</v>
+        <v>1316</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>1312</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>1313</v>
+        <v>1318</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>1314</v>
+        <v>1319</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>1315</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>1316</v>
+        <v>1321</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>587</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>1317</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14544,13 +14504,13 @@
     </row>
     <row r="314" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>1318</v>
+        <v>1323</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>1319</v>
+        <v>1324</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>1320</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14588,13 +14548,13 @@
     </row>
     <row r="318" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>1321</v>
+        <v>1326</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>1322</v>
+        <v>1327</v>
       </c>
       <c r="C318" s="3" t="s">
-        <v>1323</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14676,35 +14636,35 @@
     </row>
     <row r="326" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>1324</v>
+        <v>1329</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>1325</v>
+        <v>1330</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>1326</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>1327</v>
+        <v>1332</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>1328</v>
+        <v>1333</v>
       </c>
       <c r="C327" s="3" t="s">
-        <v>1329</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>1330</v>
+        <v>1335</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>1331</v>
+        <v>1336</v>
       </c>
       <c r="C328" s="3" t="s">
-        <v>1332</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14731,35 +14691,35 @@
     </row>
     <row r="331" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>1333</v>
+        <v>1338</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>1334</v>
+        <v>1339</v>
       </c>
       <c r="C331" s="3" t="s">
-        <v>1335</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>1336</v>
+        <v>1341</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>1337</v>
+        <v>1342</v>
       </c>
       <c r="C332" s="3" t="s">
-        <v>1338</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="6" t="s">
-        <v>1339</v>
+        <v>1344</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>1340</v>
+        <v>1345</v>
       </c>
       <c r="C333" s="7" t="s">
-        <v>1341</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14819,13 +14779,13 @@
     </row>
     <row r="339" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>1342</v>
+        <v>1347</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1343</v>
+        <v>1348</v>
       </c>
       <c r="C339" s="3" t="s">
-        <v>1344</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14841,13 +14801,13 @@
     </row>
     <row r="341" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>1345</v>
+        <v>1350</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>1346</v>
+        <v>1351</v>
       </c>
       <c r="C341" s="3" t="s">
-        <v>1347</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14874,13 +14834,13 @@
     </row>
     <row r="344" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>1348</v>
+        <v>1353</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>1349</v>
+        <v>1354</v>
       </c>
       <c r="C344" s="3" t="s">
-        <v>1350</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14896,13 +14856,13 @@
     </row>
     <row r="346" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>1351</v>
+        <v>1356</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>1352</v>
+        <v>1357</v>
       </c>
       <c r="C346" s="3" t="s">
-        <v>1353</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14951,13 +14911,13 @@
     </row>
     <row r="351" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>1354</v>
+        <v>1359</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>1355</v>
+        <v>1360</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>1356</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14973,24 +14933,24 @@
     </row>
     <row r="353" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>1357</v>
+        <v>1362</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>1358</v>
+        <v>1363</v>
       </c>
       <c r="C353" s="3" t="s">
-        <v>1359</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>1360</v>
+        <v>1365</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>1361</v>
+        <v>1366</v>
       </c>
       <c r="C354" s="3" t="s">
-        <v>1362</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15006,10 +14966,10 @@
     </row>
     <row r="356" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>1363</v>
+        <v>1368</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>1364</v>
+        <v>1369</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>697</v>
@@ -15028,40 +14988,40 @@
     </row>
     <row r="358" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>1365</v>
+        <v>1370</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>1366</v>
+        <v>1371</v>
       </c>
       <c r="C358" s="3" t="s">
-        <v>1367</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>1368</v>
+        <v>1373</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1369</v>
+        <v>1374</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>1370</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>1371</v>
+        <v>1376</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>1372</v>
+        <v>1377</v>
       </c>
       <c r="C360" s="3" t="s">
-        <v>1373</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="4" t="s">
-        <v>701</v>
+        <v>1379</v>
       </c>
       <c r="B361" s="5" t="s">
         <v>702</v>
@@ -15072,29 +15032,29 @@
     </row>
     <row r="362" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>1374</v>
+        <v>1380</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>1375</v>
+        <v>1381</v>
       </c>
       <c r="C362" s="3" t="s">
-        <v>1376</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>1377</v>
+        <v>1383</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>1378</v>
+        <v>1384</v>
       </c>
       <c r="C363" s="3" t="s">
-        <v>1379</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="4" t="s">
-        <v>704</v>
+        <v>1386</v>
       </c>
       <c r="B364" s="5" t="s">
         <v>705</v>
@@ -15116,10 +15076,10 @@
     </row>
     <row r="366" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>1380</v>
+        <v>1387</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>1381</v>
+        <v>1388</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>709</v>
@@ -15149,35 +15109,35 @@
     </row>
     <row r="369" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>1382</v>
+        <v>1389</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>1383</v>
+        <v>1390</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>1384</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>1385</v>
+        <v>1392</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>1386</v>
+        <v>1393</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>1387</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>1388</v>
+        <v>1395</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1389</v>
+        <v>1396</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>1390</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15226,24 +15186,24 @@
     </row>
     <row r="376" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1391</v>
+        <v>1398</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1392</v>
+        <v>1399</v>
       </c>
       <c r="C376" s="3" t="s">
-        <v>1393</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1394</v>
+        <v>1401</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1395</v>
+        <v>1402</v>
       </c>
       <c r="C377" s="3" t="s">
-        <v>1396</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15347,13 +15307,13 @@
     </row>
     <row r="387" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1397</v>
+        <v>1404</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1398</v>
+        <v>1405</v>
       </c>
       <c r="C387" s="3" t="s">
-        <v>1399</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15380,24 +15340,24 @@
     </row>
     <row r="390" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1400</v>
+        <v>1407</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1401</v>
+        <v>1408</v>
       </c>
       <c r="C390" s="3" t="s">
-        <v>1402</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1403</v>
+        <v>1410</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1404</v>
+        <v>1411</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>1405</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15424,35 +15384,35 @@
     </row>
     <row r="394" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1406</v>
+        <v>1413</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1407</v>
+        <v>1414</v>
       </c>
       <c r="C394" s="3" t="s">
-        <v>1408</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1409</v>
+        <v>1416</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1410</v>
+        <v>1417</v>
       </c>
       <c r="C395" s="3" t="s">
-        <v>1411</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1412</v>
+        <v>1419</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1413</v>
+        <v>1420</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>1414</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15490,62 +15450,62 @@
     </row>
     <row r="400" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1415</v>
+        <v>1422</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1416</v>
+        <v>1423</v>
       </c>
       <c r="C400" s="3" t="s">
-        <v>1417</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1418</v>
+        <v>1425</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1419</v>
+        <v>1426</v>
       </c>
       <c r="C401" s="3" t="s">
-        <v>1420</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1421</v>
+        <v>1428</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1422</v>
+        <v>1429</v>
       </c>
       <c r="C402" s="3" t="s">
-        <v>1423</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1424</v>
+        <v>1431</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1425</v>
+        <v>1432</v>
       </c>
       <c r="C403" s="3" t="s">
-        <v>1426</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1427</v>
+        <v>1434</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1428</v>
+        <v>1435</v>
       </c>
       <c r="C404" s="3" t="s">
-        <v>1429</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="4" t="s">
-        <v>1430</v>
+        <v>1437</v>
       </c>
       <c r="B405" s="5" t="s">
         <v>761</v>
@@ -15556,46 +15516,46 @@
     </row>
     <row r="406" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1431</v>
+        <v>1438</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1432</v>
+        <v>1439</v>
       </c>
       <c r="C406" s="3" t="s">
-        <v>1433</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1434</v>
+        <v>1441</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1435</v>
+        <v>1442</v>
       </c>
       <c r="C407" s="3" t="s">
-        <v>1436</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1437</v>
+        <v>1444</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1438</v>
+        <v>1445</v>
       </c>
       <c r="C408" s="3" t="s">
-        <v>1439</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1440</v>
+        <v>1447</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1441</v>
+        <v>1448</v>
       </c>
       <c r="C409" s="3" t="s">
-        <v>1442</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15611,13 +15571,13 @@
     </row>
     <row r="411" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1443</v>
+        <v>1450</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1155</v>
+        <v>1159</v>
       </c>
       <c r="C411" s="3" t="s">
-        <v>1444</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15625,285 +15585,285 @@
         <v>841</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1445</v>
+        <v>1452</v>
       </c>
       <c r="C412" s="3" t="s">
-        <v>1446</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1447</v>
+        <v>1454</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1448</v>
+        <v>1455</v>
       </c>
       <c r="C413" s="3" t="s">
-        <v>1449</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1450</v>
+        <v>1457</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1451</v>
+        <v>1458</v>
       </c>
       <c r="C414" s="3" t="s">
-        <v>1452</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1453</v>
+        <v>1460</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1454</v>
+        <v>1461</v>
       </c>
       <c r="C415" s="3" t="s">
-        <v>1455</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1456</v>
+        <v>1463</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1457</v>
+        <v>1464</v>
       </c>
       <c r="C416" s="3" t="s">
-        <v>1458</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1459</v>
+        <v>1466</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1460</v>
+        <v>1467</v>
       </c>
       <c r="C417" s="3" t="s">
-        <v>1461</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1462</v>
+        <v>1469</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1463</v>
+        <v>1470</v>
       </c>
       <c r="C418" s="3" t="s">
-        <v>1464</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1465</v>
+        <v>1472</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1466</v>
+        <v>1473</v>
       </c>
       <c r="C419" s="3" t="s">
-        <v>1467</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1468</v>
+        <v>1475</v>
       </c>
       <c r="B420" s="3" t="s">
         <v>293</v>
       </c>
       <c r="C420" s="3" t="s">
-        <v>1469</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1470</v>
+        <v>1477</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1471</v>
+        <v>1478</v>
       </c>
       <c r="C421" s="3" t="s">
-        <v>1472</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1473</v>
+        <v>1480</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1474</v>
+        <v>1481</v>
       </c>
       <c r="C422" s="3" t="s">
-        <v>1475</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1476</v>
+        <v>1483</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1477</v>
+        <v>1484</v>
       </c>
       <c r="C423" s="3" t="s">
-        <v>1478</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1479</v>
+        <v>1486</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1480</v>
+        <v>1487</v>
       </c>
       <c r="C424" s="3" t="s">
-        <v>1481</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1482</v>
+        <v>1489</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1483</v>
+        <v>1490</v>
       </c>
       <c r="C425" s="3" t="s">
-        <v>1484</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1485</v>
+        <v>1492</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1486</v>
+        <v>1493</v>
       </c>
       <c r="C426" s="3" t="s">
-        <v>1487</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1488</v>
+        <v>1495</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1489</v>
+        <v>1496</v>
       </c>
       <c r="C427" s="3" t="s">
-        <v>1490</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1491</v>
+        <v>1498</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1492</v>
+        <v>1499</v>
       </c>
       <c r="C428" s="3" t="s">
-        <v>1493</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1494</v>
+        <v>1501</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1495</v>
+        <v>1502</v>
       </c>
       <c r="C429" s="3" t="s">
-        <v>1496</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1497</v>
+        <v>1504</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1498</v>
+        <v>1505</v>
       </c>
       <c r="C430" s="3" t="s">
-        <v>1499</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1500</v>
+        <v>1507</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1501</v>
+        <v>1508</v>
       </c>
       <c r="C431" s="3" t="s">
-        <v>1502</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1503</v>
+        <v>1510</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1504</v>
+        <v>1511</v>
       </c>
       <c r="C432" s="3" t="s">
-        <v>1505</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1506</v>
+        <v>1513</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1507</v>
+        <v>1514</v>
       </c>
       <c r="C433" s="3" t="s">
-        <v>1508</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1509</v>
+        <v>1516</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1510</v>
+        <v>1517</v>
       </c>
       <c r="C434" s="3" t="s">
-        <v>1439</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1511</v>
+        <v>1518</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1512</v>
+        <v>1519</v>
       </c>
       <c r="C435" s="3" t="s">
-        <v>1513</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1514</v>
+        <v>1521</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1515</v>
+        <v>1522</v>
       </c>
       <c r="C436" s="3" t="s">
-        <v>1516</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1517</v>
+        <v>1524</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1518</v>
+        <v>1525</v>
       </c>
       <c r="C437" s="3" t="s">
-        <v>1519</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15911,76 +15871,76 @@
         <v>785</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1520</v>
+        <v>1527</v>
       </c>
       <c r="C438" s="3" t="s">
-        <v>1521</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1522</v>
+        <v>1529</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1523</v>
+        <v>1530</v>
       </c>
       <c r="C439" s="3" t="s">
-        <v>1524</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1525</v>
+        <v>1532</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1526</v>
+        <v>1533</v>
       </c>
       <c r="C440" s="3" t="s">
-        <v>1527</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1528</v>
+        <v>1535</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1529</v>
+        <v>1536</v>
       </c>
       <c r="C441" s="3" t="s">
-        <v>1530</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1531</v>
+        <v>1538</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1532</v>
+        <v>1539</v>
       </c>
       <c r="C442" s="3" t="s">
-        <v>1533</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1534</v>
+        <v>1541</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1535</v>
+        <v>1542</v>
       </c>
       <c r="C443" s="3" t="s">
-        <v>1536</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1537</v>
+        <v>1544</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1538</v>
+        <v>1545</v>
       </c>
       <c r="C444" s="3" t="s">
-        <v>1539</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16018,35 +15978,35 @@
     </row>
     <row r="448" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1540</v>
+        <v>1547</v>
       </c>
       <c r="B448" s="3" t="s">
-        <v>1541</v>
+        <v>1548</v>
       </c>
       <c r="C448" s="3" t="s">
-        <v>1542</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1543</v>
+        <v>1550</v>
       </c>
       <c r="B449" s="3" t="s">
-        <v>1544</v>
+        <v>1551</v>
       </c>
       <c r="C449" s="3" t="s">
-        <v>1545</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1546</v>
+        <v>1553</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1547</v>
+        <v>1554</v>
       </c>
       <c r="C450" s="3" t="s">
-        <v>1548</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16062,18 +16022,18 @@
     </row>
     <row r="452" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1549</v>
+        <v>1556</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1550</v>
+        <v>1557</v>
       </c>
       <c r="C452" s="3" t="s">
-        <v>1551</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="4" t="s">
-        <v>769</v>
+        <v>1559</v>
       </c>
       <c r="B453" s="5" t="s">
         <v>373</v>
@@ -16084,24 +16044,24 @@
     </row>
     <row r="454" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1552</v>
+        <v>1560</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1553</v>
+        <v>1561</v>
       </c>
       <c r="C454" s="3" t="s">
-        <v>1554</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1555</v>
+        <v>1563</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1556</v>
+        <v>1564</v>
       </c>
       <c r="C455" s="3" t="s">
-        <v>1557</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16249,24 +16209,24 @@
     </row>
     <row r="469" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1558</v>
+        <v>1566</v>
       </c>
       <c r="B469" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C469" s="3" t="s">
-        <v>1559</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1560</v>
+        <v>1568</v>
       </c>
       <c r="B470" s="3" t="s">
-        <v>1561</v>
+        <v>1569</v>
       </c>
       <c r="C470" s="3" t="s">
-        <v>1562</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16282,46 +16242,46 @@
     </row>
     <row r="472" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1563</v>
+        <v>1571</v>
       </c>
       <c r="B472" s="3" t="s">
-        <v>1564</v>
+        <v>1572</v>
       </c>
       <c r="C472" s="3" t="s">
-        <v>1565</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1566</v>
+        <v>1574</v>
       </c>
       <c r="B473" s="3" t="s">
-        <v>1567</v>
+        <v>1575</v>
       </c>
       <c r="C473" s="3" t="s">
-        <v>1568</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1569</v>
+        <v>1577</v>
       </c>
       <c r="B474" s="3" t="s">
-        <v>1570</v>
+        <v>1578</v>
       </c>
       <c r="C474" s="3" t="s">
-        <v>1571</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1572</v>
+        <v>1580</v>
       </c>
       <c r="B475" s="3" t="s">
-        <v>1573</v>
+        <v>1581</v>
       </c>
       <c r="C475" s="3" t="s">
-        <v>1574</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16337,35 +16297,35 @@
     </row>
     <row r="477" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1575</v>
+        <v>1583</v>
       </c>
       <c r="B477" s="3" t="s">
-        <v>1576</v>
+        <v>1584</v>
       </c>
       <c r="C477" s="3" t="s">
-        <v>1577</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1578</v>
+        <v>1586</v>
       </c>
       <c r="B478" s="3" t="s">
-        <v>1579</v>
+        <v>1587</v>
       </c>
       <c r="C478" s="3" t="s">
-        <v>1580</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1581</v>
+        <v>1589</v>
       </c>
       <c r="B479" s="3" t="s">
-        <v>1582</v>
+        <v>1590</v>
       </c>
       <c r="C479" s="3" t="s">
-        <v>1583</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16425,35 +16385,35 @@
     </row>
     <row r="485" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1584</v>
+        <v>1592</v>
       </c>
       <c r="B485" s="3" t="s">
-        <v>1585</v>
+        <v>1593</v>
       </c>
       <c r="C485" s="3" t="s">
-        <v>1586</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1587</v>
+        <v>1595</v>
       </c>
       <c r="B486" s="3" t="s">
-        <v>1588</v>
+        <v>1596</v>
       </c>
       <c r="C486" s="3" t="s">
-        <v>1589</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1590</v>
+        <v>1598</v>
       </c>
       <c r="B487" s="3" t="s">
-        <v>1591</v>
+        <v>1599</v>
       </c>
       <c r="C487" s="3" t="s">
-        <v>1592</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16491,101 +16451,101 @@
     </row>
     <row r="491" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1593</v>
+        <v>1601</v>
       </c>
       <c r="B491" s="3" t="s">
-        <v>1594</v>
+        <v>1602</v>
       </c>
       <c r="C491" s="3" t="s">
-        <v>1595</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1596</v>
+        <v>1604</v>
       </c>
       <c r="B492" s="3" t="s">
-        <v>1597</v>
+        <v>1605</v>
       </c>
       <c r="C492" s="3" t="s">
-        <v>1598</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1599</v>
+        <v>1607</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>1600</v>
+        <v>1608</v>
       </c>
       <c r="C493" s="3" t="s">
-        <v>1601</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1602</v>
+        <v>1610</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>1603</v>
+        <v>1611</v>
       </c>
       <c r="C494" s="3" t="s">
-        <v>1604</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1605</v>
+        <v>1613</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1279</v>
+        <v>1284</v>
       </c>
       <c r="C495" s="3" t="s">
-        <v>1606</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1607</v>
+        <v>1615</v>
       </c>
       <c r="B496" s="3" t="s">
-        <v>1608</v>
+        <v>1616</v>
       </c>
       <c r="C496" s="3" t="s">
-        <v>1609</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1610</v>
+        <v>1618</v>
       </c>
       <c r="B497" s="3" t="s">
-        <v>1611</v>
+        <v>1619</v>
       </c>
       <c r="C497" s="3" t="s">
-        <v>1612</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1613</v>
+        <v>1621</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>1614</v>
+        <v>1622</v>
       </c>
       <c r="C498" s="3" t="s">
-        <v>1615</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1616</v>
+        <v>1624</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>1617</v>
+        <v>1625</v>
       </c>
       <c r="C499" s="3" t="s">
-        <v>1618</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16601,24 +16561,24 @@
     </row>
     <row r="501" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1619</v>
+        <v>1627</v>
       </c>
       <c r="B501" s="3" t="s">
-        <v>1620</v>
+        <v>1628</v>
       </c>
       <c r="C501" s="3" t="s">
-        <v>1621</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1622</v>
+        <v>1630</v>
       </c>
       <c r="B502" s="3" t="s">
-        <v>1623</v>
+        <v>1631</v>
       </c>
       <c r="C502" s="3" t="s">
-        <v>1624</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16645,24 +16605,24 @@
     </row>
     <row r="505" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1625</v>
+        <v>1633</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1626</v>
+        <v>1634</v>
       </c>
       <c r="C505" s="3" t="s">
-        <v>1627</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1628</v>
+        <v>1636</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1629</v>
+        <v>1637</v>
       </c>
       <c r="C506" s="3" t="s">
-        <v>1630</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16689,167 +16649,167 @@
     </row>
     <row r="509" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1631</v>
+        <v>1639</v>
       </c>
       <c r="B509" s="3" t="s">
-        <v>1632</v>
+        <v>1640</v>
       </c>
       <c r="C509" s="3" t="s">
-        <v>1633</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1634</v>
+        <v>1642</v>
       </c>
       <c r="B510" s="3" t="s">
-        <v>1635</v>
+        <v>1643</v>
       </c>
       <c r="C510" s="3" t="s">
-        <v>1636</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1637</v>
+        <v>1645</v>
       </c>
       <c r="B511" s="3" t="s">
-        <v>1638</v>
+        <v>1646</v>
       </c>
       <c r="C511" s="3" t="s">
-        <v>1639</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1640</v>
+        <v>1648</v>
       </c>
       <c r="B512" s="3" t="s">
-        <v>1641</v>
+        <v>1649</v>
       </c>
       <c r="C512" s="3" t="s">
-        <v>1642</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1643</v>
+        <v>1651</v>
       </c>
       <c r="B513" s="3" t="s">
-        <v>1644</v>
+        <v>1652</v>
       </c>
       <c r="C513" s="3" t="s">
-        <v>1642</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1645</v>
+        <v>1653</v>
       </c>
       <c r="B514" s="3" t="s">
-        <v>1646</v>
+        <v>1654</v>
       </c>
       <c r="C514" s="3" t="s">
-        <v>1647</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="2" t="s">
-        <v>1648</v>
+        <v>1656</v>
       </c>
       <c r="B515" s="3" t="s">
-        <v>1649</v>
+        <v>1657</v>
       </c>
       <c r="C515" s="3" t="s">
-        <v>1650</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="2" t="s">
-        <v>1651</v>
+        <v>1659</v>
       </c>
       <c r="B516" s="3" t="s">
-        <v>1652</v>
+        <v>1660</v>
       </c>
       <c r="C516" s="3" t="s">
-        <v>1653</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="2" t="s">
-        <v>1654</v>
+        <v>1662</v>
       </c>
       <c r="B517" s="3" t="s">
-        <v>1655</v>
+        <v>1663</v>
       </c>
       <c r="C517" s="3" t="s">
-        <v>1656</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="2" t="s">
-        <v>1657</v>
+        <v>1665</v>
       </c>
       <c r="B518" s="3" t="s">
-        <v>1658</v>
+        <v>1666</v>
       </c>
       <c r="C518" s="3" t="s">
-        <v>1659</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="2" t="s">
-        <v>1660</v>
+        <v>1668</v>
       </c>
       <c r="B519" s="3" t="s">
-        <v>1661</v>
+        <v>1669</v>
       </c>
       <c r="C519" s="3" t="s">
-        <v>1662</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="2" t="s">
-        <v>1663</v>
+        <v>1671</v>
       </c>
       <c r="B520" s="3" t="s">
-        <v>1664</v>
+        <v>1672</v>
       </c>
       <c r="C520" s="3" t="s">
-        <v>1665</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="2" t="s">
-        <v>1666</v>
+        <v>1674</v>
       </c>
       <c r="B521" s="3" t="s">
-        <v>1667</v>
+        <v>1675</v>
       </c>
       <c r="C521" s="3" t="s">
-        <v>1668</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="2" t="s">
-        <v>1669</v>
+        <v>1677</v>
       </c>
       <c r="B522" s="3" t="s">
-        <v>1670</v>
+        <v>1678</v>
       </c>
       <c r="C522" s="3" t="s">
-        <v>1671</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="2" t="s">
-        <v>1672</v>
+        <v>1680</v>
       </c>
       <c r="B523" s="3" t="s">
-        <v>1673</v>
+        <v>1681</v>
       </c>
       <c r="C523" s="3" t="s">
-        <v>1674</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16876,10 +16836,10 @@
     </row>
     <row r="526" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="2" t="s">
-        <v>1675</v>
+        <v>1683</v>
       </c>
       <c r="B526" s="3" t="s">
-        <v>1676</v>
+        <v>1684</v>
       </c>
       <c r="C526" s="3" t="s">
         <v>828</v>
@@ -16898,13 +16858,13 @@
     </row>
     <row r="528" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="2" t="s">
-        <v>1677</v>
+        <v>1685</v>
       </c>
       <c r="B528" s="3" t="s">
-        <v>1678</v>
+        <v>1686</v>
       </c>
       <c r="C528" s="3" t="s">
-        <v>1679</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16942,7 +16902,7 @@
     </row>
     <row r="532" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="4" t="s">
-        <v>829</v>
+        <v>1688</v>
       </c>
       <c r="B532" s="5" t="s">
         <v>830</v>
@@ -16962,7 +16922,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="534" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="534" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="4" t="s">
         <v>835</v>
       </c>
@@ -16995,9 +16955,9 @@
         <v>843</v>
       </c>
     </row>
-    <row r="537" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="537" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="4" t="s">
-        <v>1680</v>
+        <v>1689</v>
       </c>
       <c r="B537" s="5" t="s">
         <v>287</v>
@@ -17008,10 +16968,10 @@
     </row>
     <row r="538" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="2" t="s">
-        <v>1681</v>
+        <v>1690</v>
       </c>
       <c r="B538" s="3" t="s">
-        <v>1682</v>
+        <v>1691</v>
       </c>
       <c r="C538" s="3" t="s">
         <v>845</v>
@@ -17019,13 +16979,13 @@
     </row>
     <row r="539" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="2" t="s">
-        <v>1683</v>
+        <v>1692</v>
       </c>
       <c r="B539" s="3" t="s">
-        <v>1684</v>
+        <v>1693</v>
       </c>
       <c r="C539" s="3" t="s">
-        <v>1685</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17041,46 +17001,46 @@
     </row>
     <row r="541" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="2" t="s">
-        <v>1686</v>
+        <v>1695</v>
       </c>
       <c r="B541" s="3" t="s">
-        <v>1687</v>
+        <v>1696</v>
       </c>
       <c r="C541" s="3" t="s">
-        <v>1688</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="2" t="s">
-        <v>1689</v>
+        <v>1698</v>
       </c>
       <c r="B542" s="3" t="s">
-        <v>1690</v>
+        <v>1699</v>
       </c>
       <c r="C542" s="3" t="s">
-        <v>1691</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="2" t="s">
-        <v>1692</v>
+        <v>1701</v>
       </c>
       <c r="B543" s="3" t="s">
-        <v>1693</v>
+        <v>1702</v>
       </c>
       <c r="C543" s="3" t="s">
-        <v>1694</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="2" t="s">
-        <v>1695</v>
+        <v>1704</v>
       </c>
       <c r="B544" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C544" s="3" t="s">
-        <v>1694</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17096,10 +17056,10 @@
     </row>
     <row r="546" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="2" t="s">
-        <v>1696</v>
+        <v>1705</v>
       </c>
       <c r="B546" s="3" t="s">
-        <v>1697</v>
+        <v>1706</v>
       </c>
       <c r="C546" s="3" t="s">
         <v>458</v>
@@ -17107,7 +17067,7 @@
     </row>
     <row r="547" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="4" t="s">
-        <v>852</v>
+        <v>1707</v>
       </c>
       <c r="B547" s="5" t="s">
         <v>853</v>
@@ -17118,29 +17078,29 @@
     </row>
     <row r="548" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="2" t="s">
-        <v>1698</v>
+        <v>1708</v>
       </c>
       <c r="B548" s="3" t="s">
-        <v>1699</v>
+        <v>1709</v>
       </c>
       <c r="C548" s="3" t="s">
-        <v>1700</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="2" t="s">
-        <v>1701</v>
+        <v>1711</v>
       </c>
       <c r="B549" s="3" t="s">
-        <v>1702</v>
+        <v>1712</v>
       </c>
       <c r="C549" s="3" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="550" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="4" t="s">
-        <v>1704</v>
+        <v>1714</v>
       </c>
       <c r="B550" s="5" t="s">
         <v>856</v>
@@ -17151,18 +17111,18 @@
     </row>
     <row r="551" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="2" t="s">
-        <v>1705</v>
+        <v>1715</v>
       </c>
       <c r="B551" s="3" t="s">
-        <v>1706</v>
+        <v>1716</v>
       </c>
       <c r="C551" s="3" t="s">
-        <v>1707</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="4" t="s">
-        <v>858</v>
+        <v>1718</v>
       </c>
       <c r="B552" s="5" t="s">
         <v>859</v>
@@ -17173,24 +17133,24 @@
     </row>
     <row r="553" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="2" t="s">
-        <v>1708</v>
+        <v>1719</v>
       </c>
       <c r="B553" s="3" t="s">
-        <v>1709</v>
+        <v>1720</v>
       </c>
       <c r="C553" s="3" t="s">
-        <v>1710</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="2" t="s">
-        <v>1711</v>
+        <v>1722</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>1712</v>
+        <v>1723</v>
       </c>
       <c r="C554" s="3" t="s">
-        <v>1713</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17206,73 +17166,73 @@
     </row>
     <row r="556" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="2" t="s">
-        <v>1714</v>
+        <v>1725</v>
       </c>
       <c r="B556" s="3" t="s">
-        <v>1715</v>
+        <v>1726</v>
       </c>
       <c r="C556" s="3" t="s">
-        <v>1716</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="2" t="s">
-        <v>1717</v>
+        <v>1728</v>
       </c>
       <c r="B557" s="3" t="s">
-        <v>1718</v>
+        <v>1729</v>
       </c>
       <c r="C557" s="3" t="s">
-        <v>1719</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="2" t="s">
-        <v>1720</v>
+        <v>1731</v>
       </c>
       <c r="B558" s="3" t="s">
-        <v>1721</v>
+        <v>1732</v>
       </c>
       <c r="C558" s="3" t="s">
-        <v>1722</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="2" t="s">
-        <v>1723</v>
+        <v>1734</v>
       </c>
       <c r="B559" s="3" t="s">
-        <v>1724</v>
+        <v>1735</v>
       </c>
       <c r="C559" s="3" t="s">
-        <v>1725</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="2" t="s">
-        <v>1726</v>
+        <v>1737</v>
       </c>
       <c r="B560" s="3" t="s">
-        <v>1727</v>
+        <v>1738</v>
       </c>
       <c r="C560" s="3" t="s">
-        <v>1728</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="2" t="s">
-        <v>1729</v>
+        <v>1740</v>
       </c>
       <c r="B561" s="3" t="s">
-        <v>1730</v>
+        <v>1741</v>
       </c>
       <c r="C561" s="3" t="s">
-        <v>1731</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="4" t="s">
-        <v>864</v>
+        <v>1743</v>
       </c>
       <c r="B562" s="5" t="s">
         <v>865</v>
@@ -17281,9 +17241,9 @@
         <v>866</v>
       </c>
     </row>
-    <row r="563" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="563" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="4" t="s">
-        <v>1732</v>
+        <v>1744</v>
       </c>
       <c r="B563" s="5" t="s">
         <v>868</v>
@@ -17292,9 +17252,9 @@
         <v>869</v>
       </c>
     </row>
-    <row r="564" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="564" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="4" t="s">
-        <v>1733</v>
+        <v>1745</v>
       </c>
       <c r="B564" s="5" t="s">
         <v>871</v>
@@ -17316,90 +17276,90 @@
     </row>
     <row r="566" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="2" t="s">
-        <v>1734</v>
+        <v>1746</v>
       </c>
       <c r="B566" s="3" t="s">
-        <v>1735</v>
+        <v>1747</v>
       </c>
       <c r="C566" s="3" t="s">
-        <v>1736</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="2" t="s">
-        <v>1737</v>
+        <v>1749</v>
       </c>
       <c r="B567" s="3" t="s">
-        <v>1738</v>
+        <v>1750</v>
       </c>
       <c r="C567" s="3" t="s">
-        <v>1739</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="2" t="s">
-        <v>1740</v>
+        <v>1752</v>
       </c>
       <c r="B568" s="3" t="s">
         <v>428</v>
       </c>
       <c r="C568" s="3" t="s">
-        <v>1741</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="2" t="s">
-        <v>1742</v>
+        <v>1754</v>
       </c>
       <c r="B569" s="3" t="s">
-        <v>1743</v>
+        <v>1755</v>
       </c>
       <c r="C569" s="3" t="s">
-        <v>1744</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="2" t="s">
-        <v>1745</v>
+        <v>1757</v>
       </c>
       <c r="B570" s="3" t="s">
-        <v>1746</v>
+        <v>1758</v>
       </c>
       <c r="C570" s="3" t="s">
-        <v>1747</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="2" t="s">
-        <v>1748</v>
+        <v>1760</v>
       </c>
       <c r="B571" s="3" t="s">
         <v>868</v>
       </c>
       <c r="C571" s="3" t="s">
-        <v>1749</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="2" t="s">
-        <v>1750</v>
+        <v>1762</v>
       </c>
       <c r="B572" s="3" t="s">
-        <v>1751</v>
+        <v>1763</v>
       </c>
       <c r="C572" s="3" t="s">
-        <v>1752</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="2" t="s">
-        <v>1753</v>
+        <v>1765</v>
       </c>
       <c r="B573" s="3" t="s">
-        <v>1754</v>
+        <v>1766</v>
       </c>
       <c r="C573" s="3" t="s">
-        <v>1755</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17426,7 +17386,7 @@
     </row>
     <row r="576" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="2" t="s">
-        <v>1756</v>
+        <v>1768</v>
       </c>
       <c r="B576" s="3" t="s">
         <v>414</v>
@@ -17503,13 +17463,13 @@
     </row>
     <row r="583" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="2" t="s">
-        <v>1757</v>
+        <v>1769</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1758</v>
+        <v>1770</v>
       </c>
       <c r="C583" s="3" t="s">
-        <v>1759</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17536,13 +17496,13 @@
     </row>
     <row r="586" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="2" t="s">
-        <v>1760</v>
+        <v>1772</v>
       </c>
       <c r="B586" s="3" t="s">
-        <v>1761</v>
+        <v>1773</v>
       </c>
       <c r="C586" s="3" t="s">
-        <v>1762</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="587" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17569,57 +17529,57 @@
     </row>
     <row r="589" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="2" t="s">
-        <v>1763</v>
+        <v>1775</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1764</v>
+        <v>1776</v>
       </c>
       <c r="C589" s="3" t="s">
-        <v>1765</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="590" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="2" t="s">
-        <v>1766</v>
+        <v>1778</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1767</v>
+        <v>1779</v>
       </c>
       <c r="C590" s="3" t="s">
-        <v>1765</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="2" t="s">
-        <v>1768</v>
+        <v>1780</v>
       </c>
       <c r="B591" s="3" t="s">
-        <v>1769</v>
+        <v>1781</v>
       </c>
       <c r="C591" s="3" t="s">
-        <v>1770</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="592" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="2" t="s">
-        <v>1771</v>
+        <v>1783</v>
       </c>
       <c r="B592" s="3" t="s">
-        <v>1772</v>
+        <v>1784</v>
       </c>
       <c r="C592" s="3" t="s">
-        <v>1773</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="2" t="s">
-        <v>1774</v>
+        <v>1786</v>
       </c>
       <c r="B593" s="3" t="s">
-        <v>1775</v>
+        <v>1787</v>
       </c>
       <c r="C593" s="3" t="s">
-        <v>1776</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="594" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17671,7 +17631,7 @@
         <v>439</v>
       </c>
       <c r="B598" s="5" t="s">
-        <v>1777</v>
+        <v>1789</v>
       </c>
       <c r="C598" s="5" t="s">
         <v>441</v>
@@ -17701,13 +17661,13 @@
     </row>
     <row r="601" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="2" t="s">
-        <v>1778</v>
+        <v>1790</v>
       </c>
       <c r="B601" s="3" t="s">
-        <v>1779</v>
+        <v>1791</v>
       </c>
       <c r="C601" s="3" t="s">
-        <v>1780</v>
+        <v>1792</v>
       </c>
     </row>
   </sheetData>
@@ -17728,7 +17688,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -17741,7 +17701,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1144</v>
+        <v>1148</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -17749,34 +17709,34 @@
     </row>
     <row r="2" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>1781</v>
+        <v>1793</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1782</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>1783</v>
+        <v>1795</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1784</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>1758</v>
+        <v>1770</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1785</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>1786</v>
+        <v>1798</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1787</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17909,13 +17869,13 @@
     </row>
     <row r="9" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>1788</v>
+        <v>1800</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1789</v>
+        <v>1801</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1790</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>